<commit_message>
profile Excel file generation
</commit_message>
<xml_diff>
--- a/test/integration/TestAccs.xlsx
+++ b/test/integration/TestAccs.xlsx
@@ -395,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,78 +483,30 @@
     <row r="10" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-    </row>
-    <row r="36" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-    </row>
+    <row r="13" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>